<commit_message>
update low power software
</commit_message>
<xml_diff>
--- a/Docs/WateringSystemCalc.xlsx
+++ b/Docs/WateringSystemCalc.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2906AEC4-BAF6-4BEC-8A13-9CC7FE3A84EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB1CBB4-814C-406A-8015-E796610720CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="12825" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Power" sheetId="2" r:id="rId1"/>
+    <sheet name="Ruler_Sensor" sheetId="3" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,44 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>R</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>hmax</t>
-  </si>
-  <si>
-    <t>radius</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>res_W</t>
-  </si>
-  <si>
-    <t>res</t>
-  </si>
-  <si>
-    <t>Rw</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -76,6 +42,45 @@
   </si>
   <si>
     <t>ro</t>
+  </si>
+  <si>
+    <t>Battery_V [V]</t>
+  </si>
+  <si>
+    <t>Battery_P_max [Wh]</t>
+  </si>
+  <si>
+    <t>I_idle[A]</t>
+  </si>
+  <si>
+    <t>I_normal[A]</t>
+  </si>
+  <si>
+    <t>I_avg [A]</t>
+  </si>
+  <si>
+    <t>V_supply [V]</t>
+  </si>
+  <si>
+    <t>Battery_cap [Ah]</t>
+  </si>
+  <si>
+    <t>P_avg[W]</t>
+  </si>
+  <si>
+    <t>SMPS_eff[%]</t>
+  </si>
+  <si>
+    <t>P_in[W]</t>
+  </si>
+  <si>
+    <t>Bat_lifetime [h]</t>
+  </si>
+  <si>
+    <t>normal_on_time [m]</t>
+  </si>
+  <si>
+    <t>idle_time [m]</t>
   </si>
 </sst>
 </file>
@@ -168,54 +173,24 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>[1]Sheet2!$A$2:$A$16</c:f>
+              <c:f>#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.15</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet2!$E$2:$E$16</c:f>
+              <c:f>#REF!</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8155555.555555555</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>878846.15384615387</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>437547.89272030647</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>327023.31961591222</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>110171.6738197425</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>68457.300275482092</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1002,62 +977,9 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
-      <sheetName val="Sheet1 (2)"/>
-      <sheetName val="Sheet2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2">
-            <v>1E-3</v>
-          </cell>
-          <cell r="E2">
-            <v>8155555.555555555</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>0.01</v>
-          </cell>
-          <cell r="E3">
-            <v>878846.15384615387</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>0.02</v>
-          </cell>
-          <cell r="E4">
-            <v>437547.89272030647</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>0.03</v>
-          </cell>
-          <cell r="E5">
-            <v>327023.31961591222</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>0.1</v>
-          </cell>
-          <cell r="E6">
-            <v>110171.6738197425</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>0.15</v>
-          </cell>
-          <cell r="E7">
-            <v>68457.300275482092</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1383,118 +1305,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5370E2-3D9F-485A-B883-DED95A8B1053}">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C1">
+        <f>550/1000</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
       <c r="B2" s="1">
-        <f>B1*C2/(C1-C2)</f>
-        <v>250</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
-        <f>(C3*(B1+B2)-C1*(B2))/(C1-C3)</f>
-        <v>416.66666666666669</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <f>(C4*(B1+B2+B3)-C1*(B2+B3))/(C1-C4)</f>
-        <v>833.33333333333303</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <f>B2*B1</f>
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <f>6*60</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <f>(B5*B7 + B6*B8)/(B7+B8)</f>
+        <v>2.2849473684210527E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
-        <f>(C5*(B1+B2+B3+B4)-C1*(B2+B3+B4))/(C1-C5)</f>
-        <v>2500.0000000000009</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <f>PI()*B9^2</f>
-        <v>0.11341149479459153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <f>B11/B10*B8</f>
-        <v>10580.938044890549</v>
+        <f>B9*B10</f>
+        <v>0.11424736842105264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <f>B11/B13</f>
+        <v>0.12694152046783627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <f>B3/B14</f>
+        <v>38.994333625097894</v>
       </c>
     </row>
   </sheetData>
@@ -1503,136 +1441,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5370E2-3D9F-485A-B883-DED95A8B1053}">
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>65000</v>
-      </c>
-      <c r="C1">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1">
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1">
-        <f>(C2*(2*E1*B1)-E1^2*(C1-C2))/(E1*(C1-C2)-C2*B1)</f>
-        <v>-1056000</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <f>(C3*(B1+B2)-C1*(B2))/(C1-C3)</f>
-        <v>1099333.3333333333</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <f>(C4*(B1+B2+B3)-C1*(B2+B3))/(C1-C4)</f>
-        <v>54166.666666666744</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <f>(C5*(B1+B2+B3+B4)-C1*(B2+B3+B4))/(C1-C5)</f>
-        <v>162500</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <f>PI()*B9^2</f>
-        <v>0.11341149479459153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <f>B11/B10*B8</f>
-        <v>10580.938044890549</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00D4E5C-0FAC-4768-B8ED-95B929C74C7A}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1640,19 +1452,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>